<commit_message>
voilà une courbe qui se rapproche un peu plus de ce que je pensais
</commit_message>
<xml_diff>
--- a/1_Propulsion/Courbe accélération rush.xlsx
+++ b/1_Propulsion/Courbe accélération rush.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SVN\1_Propulsion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\clubRobot\CodeSource\1_Propulsion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -221,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -257,6 +257,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -275,7 +276,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
@@ -381,42 +382,47 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="400"/>
                 <c:pt idx="0">
-                  <c:v>3375.0000000000005</c:v>
+                  <c:v>5371.09375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2625</c:v>
+                  <c:v>4082.03125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2000</c:v>
+                  <c:v>3007.8125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1875</c:v>
+                  <c:v>2470.703125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1875</c:v>
+                  <c:v>2202.1484375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1875</c:v>
+                  <c:v>2148.4375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1875</c:v>
+                  <c:v>2148.4375</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1875</c:v>
+                  <c:v>2148.4375</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1875</c:v>
+                  <c:v>2148.4375</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1875</c:v>
+                  <c:v>2148.4375</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1875</c:v>
+                  <c:v>2148.4375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C3F6-47CF-B3DF-3A8E11C65FD9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -473,6 +479,11 @@
             </c:numLit>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C3F6-47CF-B3DF-3A8E11C65FD9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -800,7 +811,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
@@ -906,42 +917,47 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="400"/>
                 <c:pt idx="0">
-                  <c:v>345.6</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>268.8</c:v>
+                  <c:v>418</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>204.8</c:v>
+                  <c:v>308</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>192</c:v>
+                  <c:v>253</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>192</c:v>
+                  <c:v>225.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>192</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>192</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>192</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>192</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>192</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>192</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-031B-43CE-BD54-46C5E199C2A0}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -998,6 +1014,11 @@
             </c:numLit>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-031B-43CE-BD54-46C5E199C2A0}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2762,8 +2783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD228"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2772,8 +2793,8 @@
     <col min="3" max="3" width="12.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="3.85546875" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56" x14ac:dyDescent="0.25">
@@ -2908,7 +2929,7 @@
       </c>
       <c r="C3" s="2">
         <f>I5*H8</f>
-        <v>345.6</v>
+        <v>550</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="19"/>
@@ -2925,7 +2946,7 @@
       </c>
       <c r="N3" s="2">
         <f>C3/4096/25*1000*1000</f>
-        <v>3375.0000000000005</v>
+        <v>5371.09375</v>
       </c>
       <c r="O3" s="19"/>
       <c r="P3" s="10"/>
@@ -2978,11 +2999,11 @@
       </c>
       <c r="C4" s="2">
         <f>IF(C3-$I$5*D4 &gt; $I$5, C3-$I$5*D4, $I$5)</f>
-        <v>268.8</v>
+        <v>418</v>
       </c>
       <c r="D4" s="3">
         <f>H9</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="5" t="s">
@@ -3009,7 +3030,7 @@
       </c>
       <c r="N4" s="2">
         <f>C4/4096/25*1000*1000</f>
-        <v>2625</v>
+        <v>4082.03125</v>
       </c>
       <c r="O4" s="11"/>
       <c r="P4" s="5"/>
@@ -3057,16 +3078,16 @@
     <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="2">
-        <f>B4+$I$6/10</f>
+        <f t="shared" ref="B5:B13" si="0">B4+$I$6/10</f>
         <v>7372.8</v>
       </c>
       <c r="C5" s="2">
         <f>IF(C4-$I$5*D5 &gt; $I$5, C4-$I$5*D5, $I$5)</f>
-        <v>204.8</v>
+        <v>308</v>
       </c>
       <c r="D5" s="3">
         <f>D4/$H$10</f>
-        <v>0.33333333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="5" t="s">
@@ -3075,25 +3096,25 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5">
-        <v>192</v>
+        <v>220</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>2</v>
       </c>
       <c r="K5" s="7">
         <f>I5/4096/25*1000*1000</f>
-        <v>1875</v>
+        <v>2148.4375</v>
       </c>
       <c r="L5" s="9" t="s">
         <v>5</v>
       </c>
       <c r="M5" s="3">
-        <f t="shared" ref="M5:M14" si="0">B5/4096*1000/5</f>
+        <f t="shared" ref="M5:M13" si="1">B5/4096*1000/5</f>
         <v>360</v>
       </c>
       <c r="N5" s="2">
-        <f t="shared" ref="N5:N13" si="1">C5/4096/25*1000*1000</f>
-        <v>2000</v>
+        <f t="shared" ref="N5:N13" si="2">C5/4096/25*1000*1000</f>
+        <v>3007.8125</v>
       </c>
       <c r="O5" s="11"/>
       <c r="P5" s="5"/>
@@ -3141,16 +3162,16 @@
     <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="2">
-        <f>B5+$I$6/10</f>
+        <f t="shared" si="0"/>
         <v>11059.2</v>
       </c>
       <c r="C6" s="2">
-        <f t="shared" ref="C6:C13" si="2">IF(C5-$I$5*D6 &gt; $I$5, C5-$I$5*D6, $I$5)</f>
-        <v>192</v>
+        <f t="shared" ref="C6:C13" si="3">IF(C5-$I$5*D6 &gt; $I$5, C5-$I$5*D6, $I$5)</f>
+        <v>253</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" ref="D6:D13" si="3">D5/2</f>
-        <v>0.16666666666666669</v>
+        <f t="shared" ref="D6:D13" si="4">D5/2</f>
+        <v>0.25</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="5" t="s">
@@ -3172,12 +3193,12 @@
         <v>6</v>
       </c>
       <c r="M6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>540</v>
       </c>
       <c r="N6" s="2">
-        <f t="shared" si="1"/>
-        <v>1875</v>
+        <f t="shared" si="2"/>
+        <v>2470.703125</v>
       </c>
       <c r="O6" s="11"/>
       <c r="P6" s="5"/>
@@ -3225,16 +3246,16 @@
     <row r="7" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="2">
-        <f>B6+$I$6/10</f>
+        <f t="shared" si="0"/>
         <v>14745.6</v>
       </c>
       <c r="C7" s="2">
-        <f t="shared" si="2"/>
-        <v>192</v>
+        <f t="shared" si="3"/>
+        <v>225.5</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="3"/>
-        <v>8.3333333333333343E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.125</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="5"/>
@@ -3245,12 +3266,12 @@
       <c r="K7" s="5"/>
       <c r="L7" s="9"/>
       <c r="M7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>720</v>
       </c>
       <c r="N7" s="2">
-        <f t="shared" si="1"/>
-        <v>1875</v>
+        <f t="shared" si="2"/>
+        <v>2202.1484375</v>
       </c>
       <c r="O7" s="11"/>
       <c r="P7" s="5"/>
@@ -3298,16 +3319,16 @@
     <row r="8" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="2">
-        <f>B7+$I$6/10</f>
+        <f t="shared" si="0"/>
         <v>18432</v>
       </c>
       <c r="C8" s="2">
-        <f t="shared" si="2"/>
-        <v>192</v>
+        <f t="shared" si="3"/>
+        <v>220</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" si="3"/>
-        <v>4.1666666666666671E-2</v>
+        <f t="shared" si="4"/>
+        <v>6.25E-2</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="5" t="s">
@@ -3315,19 +3336,19 @@
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5">
-        <v>1.8</v>
+        <v>2.5</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="9"/>
       <c r="M8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>900</v>
       </c>
       <c r="N8" s="2">
-        <f t="shared" si="1"/>
-        <v>1875</v>
+        <f t="shared" si="2"/>
+        <v>2148.4375</v>
       </c>
       <c r="O8" s="11"/>
       <c r="P8" s="5"/>
@@ -3375,36 +3396,36 @@
     <row r="9" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="2">
-        <f>B8+$I$6/10</f>
+        <f t="shared" si="0"/>
         <v>22118.400000000001</v>
       </c>
       <c r="C9" s="2">
-        <f t="shared" si="2"/>
-        <v>192</v>
+        <f t="shared" si="3"/>
+        <v>220</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" si="3"/>
-        <v>2.0833333333333336E-2</v>
+        <f t="shared" si="4"/>
+        <v>3.125E-2</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="5"/>
-      <c r="H9" s="5">
-        <v>0.4</v>
+      <c r="H9" s="25">
+        <v>0.6</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="9"/>
       <c r="M9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1080</v>
       </c>
       <c r="N9" s="2">
-        <f t="shared" si="1"/>
-        <v>1875</v>
+        <f t="shared" si="2"/>
+        <v>2148.4375</v>
       </c>
       <c r="O9" s="11"/>
       <c r="P9" s="5"/>
@@ -3452,16 +3473,16 @@
     <row r="10" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="2">
-        <f>B9+$I$6/10</f>
+        <f t="shared" si="0"/>
         <v>25804.800000000003</v>
       </c>
       <c r="C10" s="2">
-        <f t="shared" si="2"/>
-        <v>192</v>
+        <f t="shared" si="3"/>
+        <v>220</v>
       </c>
       <c r="D10" s="3">
-        <f t="shared" si="3"/>
-        <v>1.0416666666666668E-2</v>
+        <f t="shared" si="4"/>
+        <v>1.5625E-2</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="5" t="s">
@@ -3476,12 +3497,12 @@
       <c r="K10" s="5"/>
       <c r="L10" s="9"/>
       <c r="M10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1260.0000000000002</v>
       </c>
       <c r="N10" s="2">
-        <f t="shared" si="1"/>
-        <v>1875</v>
+        <f t="shared" si="2"/>
+        <v>2148.4375</v>
       </c>
       <c r="O10" s="11"/>
       <c r="P10" s="5"/>
@@ -3529,16 +3550,16 @@
     <row r="11" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="2">
-        <f>B10+$I$6/10</f>
+        <f t="shared" si="0"/>
         <v>29491.200000000004</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="2"/>
-        <v>192</v>
+        <f t="shared" si="3"/>
+        <v>220</v>
       </c>
       <c r="D11" s="3">
-        <f t="shared" si="3"/>
-        <v>5.2083333333333339E-3</v>
+        <f t="shared" si="4"/>
+        <v>7.8125E-3</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="5"/>
@@ -3549,12 +3570,12 @@
       <c r="K11" s="5"/>
       <c r="L11" s="9"/>
       <c r="M11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1440.0000000000002</v>
       </c>
       <c r="N11" s="2">
-        <f t="shared" si="1"/>
-        <v>1875</v>
+        <f t="shared" si="2"/>
+        <v>2148.4375</v>
       </c>
       <c r="O11" s="11"/>
       <c r="P11" s="5"/>
@@ -3602,16 +3623,16 @@
     <row r="12" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="2">
-        <f>B11+$I$6/10</f>
+        <f t="shared" si="0"/>
         <v>33177.600000000006</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" si="2"/>
-        <v>192</v>
+        <f t="shared" si="3"/>
+        <v>220</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" si="3"/>
-        <v>2.604166666666667E-3</v>
+        <f t="shared" si="4"/>
+        <v>3.90625E-3</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="5"/>
@@ -3622,12 +3643,12 @@
       <c r="K12" s="5"/>
       <c r="L12" s="9"/>
       <c r="M12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1620.0000000000005</v>
       </c>
       <c r="N12" s="2">
-        <f t="shared" si="1"/>
-        <v>1875</v>
+        <f t="shared" si="2"/>
+        <v>2148.4375</v>
       </c>
       <c r="O12" s="11"/>
       <c r="P12" s="5"/>
@@ -3675,16 +3696,16 @@
     <row r="13" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="2">
-        <f>B12+$I$6/10</f>
+        <f t="shared" si="0"/>
         <v>36864.000000000007</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="2"/>
-        <v>192</v>
+        <f t="shared" si="3"/>
+        <v>220</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" si="3"/>
-        <v>1.3020833333333335E-3</v>
+        <f t="shared" si="4"/>
+        <v>1.953125E-3</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="8"/>
@@ -3695,12 +3716,12 @@
       <c r="K13" s="8"/>
       <c r="L13" s="14"/>
       <c r="M13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1800.0000000000005</v>
       </c>
       <c r="N13" s="2">
-        <f t="shared" si="1"/>
-        <v>1875</v>
+        <f t="shared" si="2"/>
+        <v>2148.4375</v>
       </c>
       <c r="O13" s="11"/>
       <c r="P13" s="5"/>
@@ -14420,7 +14441,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>